<commit_message>
new naming convention for dipoles in bo and si.
</commit_message>
<xml_diff>
--- a/excel-files/naming-service/BO-MA-PM.xlsx
+++ b/excel-files/naming-service/BO-MA-PM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="123">
   <si>
     <t>Super Section</t>
   </si>
@@ -41,7 +41,7 @@
     <t>BO</t>
   </si>
   <si>
-    <t>01</t>
+    <t>01D</t>
   </si>
   <si>
     <t>MA</t>
@@ -50,21 +50,18 @@
     <t>B</t>
   </si>
   <si>
+    <t>01U</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
     <t>QF</t>
   </si>
   <si>
-    <t>01U</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
     <t>02D</t>
   </si>
   <si>
@@ -80,7 +77,7 @@
     <t>SF</t>
   </si>
   <si>
-    <t>03</t>
+    <t>03D</t>
   </si>
   <si>
     <t>03U</t>
@@ -89,357 +86,282 @@
     <t>SD</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>04D</t>
   </si>
   <si>
     <t>04U</t>
   </si>
   <si>
-    <t>05</t>
+    <t>05D</t>
   </si>
   <si>
     <t>05U</t>
   </si>
   <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>06D</t>
   </si>
   <si>
     <t>06U</t>
   </si>
   <si>
-    <t>07</t>
+    <t>07D</t>
   </si>
   <si>
     <t>07U</t>
   </si>
   <si>
-    <t>08</t>
-  </si>
-  <si>
     <t>08D</t>
   </si>
   <si>
     <t>08U</t>
   </si>
   <si>
-    <t>09</t>
+    <t>09D</t>
   </si>
   <si>
     <t>09U</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>10D</t>
   </si>
   <si>
     <t>10U</t>
   </si>
   <si>
-    <t>11</t>
+    <t>11D</t>
   </si>
   <si>
     <t>11U</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>12D</t>
   </si>
   <si>
     <t>12U</t>
   </si>
   <si>
-    <t>13</t>
+    <t>13D</t>
   </si>
   <si>
     <t>13U</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>14D</t>
   </si>
   <si>
     <t>14U</t>
   </si>
   <si>
-    <t>15</t>
+    <t>15D</t>
   </si>
   <si>
     <t>15U</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>16D</t>
   </si>
   <si>
     <t>16U</t>
   </si>
   <si>
-    <t>17</t>
+    <t>17D</t>
   </si>
   <si>
     <t>17U</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>18D</t>
   </si>
   <si>
     <t>18U</t>
   </si>
   <si>
-    <t>19</t>
+    <t>19D</t>
   </si>
   <si>
     <t>19U</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>20D</t>
   </si>
   <si>
     <t>20U</t>
   </si>
   <si>
-    <t>21</t>
+    <t>21D</t>
   </si>
   <si>
     <t>21U</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>22D</t>
   </si>
   <si>
     <t>22U</t>
   </si>
   <si>
-    <t>23</t>
+    <t>23D</t>
   </si>
   <si>
     <t>23U</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>24D</t>
   </si>
   <si>
     <t>24U</t>
   </si>
   <si>
-    <t>25</t>
+    <t>25D</t>
   </si>
   <si>
     <t>25U</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>26D</t>
   </si>
   <si>
     <t>26U</t>
   </si>
   <si>
-    <t>27</t>
+    <t>27D</t>
   </si>
   <si>
     <t>27U</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>28D</t>
   </si>
   <si>
     <t>28U</t>
   </si>
   <si>
-    <t>29</t>
+    <t>29D</t>
   </si>
   <si>
     <t>29U</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>30D</t>
   </si>
   <si>
     <t>30U</t>
   </si>
   <si>
-    <t>31</t>
+    <t>31D</t>
   </si>
   <si>
     <t>31U</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>32D</t>
   </si>
   <si>
     <t>32U</t>
   </si>
   <si>
-    <t>33</t>
+    <t>33D</t>
   </si>
   <si>
     <t>33U</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
     <t>34D</t>
   </si>
   <si>
     <t>34U</t>
   </si>
   <si>
-    <t>35</t>
+    <t>35D</t>
   </si>
   <si>
     <t>35U</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>36D</t>
   </si>
   <si>
     <t>36U</t>
   </si>
   <si>
-    <t>37</t>
+    <t>37D</t>
   </si>
   <si>
     <t>37U</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
     <t>38D</t>
   </si>
   <si>
     <t>38U</t>
   </si>
   <si>
-    <t>39</t>
+    <t>39D</t>
   </si>
   <si>
     <t>39U</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>40D</t>
   </si>
   <si>
     <t>40U</t>
   </si>
   <si>
-    <t>41</t>
+    <t>41D</t>
   </si>
   <si>
     <t>41U</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>42D</t>
   </si>
   <si>
     <t>42U</t>
   </si>
   <si>
-    <t>43</t>
+    <t>43D</t>
   </si>
   <si>
     <t>43U</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
     <t>44D</t>
   </si>
   <si>
     <t>44U</t>
   </si>
   <si>
-    <t>45</t>
+    <t>45D</t>
   </si>
   <si>
     <t>45U</t>
   </si>
   <si>
-    <t>46</t>
-  </si>
-  <si>
     <t>46D</t>
   </si>
   <si>
     <t>46U</t>
   </si>
   <si>
-    <t>47</t>
+    <t>47D</t>
   </si>
   <si>
     <t>47U</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>48D</t>
   </si>
   <si>
     <t>48U</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
     <t>49D</t>
   </si>
   <si>
     <t>49U</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>50D</t>
   </si>
   <si>
@@ -453,9 +375,6 @@
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>01D</t>
   </si>
   <si>
     <t>PM</t>
@@ -589,8 +508,8 @@
   </sheetPr>
   <dimension ref="A1:H220"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A187" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F216" activeCellId="0" sqref="F216"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J216" activeCellId="0" sqref="J216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -641,13 +560,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -656,7 +575,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
@@ -671,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
@@ -707,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -716,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
@@ -731,13 +650,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F9" s="4"/>
     </row>
@@ -746,13 +665,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -761,7 +680,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>9</v>
@@ -782,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -791,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>9</v>
@@ -806,7 +725,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>9</v>
@@ -821,13 +740,13 @@
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -836,7 +755,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>9</v>
@@ -851,13 +770,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -866,13 +785,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F18" s="4"/>
     </row>
@@ -881,13 +800,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4"/>
     </row>
@@ -896,7 +815,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>9</v>
@@ -911,13 +830,13 @@
         <v>7</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" s="4"/>
     </row>
@@ -926,7 +845,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>9</v>
@@ -941,7 +860,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>9</v>
@@ -956,7 +875,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>9</v>
@@ -971,13 +890,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F25" s="4"/>
     </row>
@@ -986,13 +905,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F26" s="4"/>
     </row>
@@ -1001,13 +920,13 @@
         <v>7</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="4"/>
     </row>
@@ -1016,7 +935,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>9</v>
@@ -1031,13 +950,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" s="4"/>
     </row>
@@ -1046,7 +965,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>9</v>
@@ -1061,7 +980,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>9</v>
@@ -1076,7 +995,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>9</v>
@@ -1091,13 +1010,13 @@
         <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F33" s="4"/>
     </row>
@@ -1106,13 +1025,13 @@
         <v>7</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F34" s="4"/>
     </row>
@@ -1121,13 +1040,13 @@
         <v>7</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F35" s="4"/>
     </row>
@@ -1136,13 +1055,13 @@
         <v>7</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F36" s="4"/>
     </row>
@@ -1151,7 +1070,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>9</v>
@@ -1166,13 +1085,13 @@
         <v>7</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F38" s="4"/>
     </row>
@@ -1181,7 +1100,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
@@ -1196,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -1211,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
@@ -1226,13 +1145,13 @@
         <v>7</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F42" s="4"/>
     </row>
@@ -1241,13 +1160,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F43" s="4"/>
     </row>
@@ -1256,13 +1175,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F44" s="4"/>
     </row>
@@ -1271,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>9</v>
@@ -1286,13 +1205,13 @@
         <v>7</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F46" s="4"/>
     </row>
@@ -1301,7 +1220,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>9</v>
@@ -1316,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>9</v>
@@ -1331,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>9</v>
@@ -1346,13 +1265,13 @@
         <v>7</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F50" s="4"/>
     </row>
@@ -1361,13 +1280,13 @@
         <v>7</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F51" s="4"/>
     </row>
@@ -1376,13 +1295,13 @@
         <v>7</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F52" s="4"/>
     </row>
@@ -1391,7 +1310,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
@@ -1406,13 +1325,13 @@
         <v>7</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F54" s="4"/>
     </row>
@@ -1421,7 +1340,7 @@
         <v>7</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>9</v>
@@ -1436,7 +1355,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>9</v>
@@ -1451,13 +1370,13 @@
         <v>7</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F57" s="4"/>
     </row>
@@ -1466,7 +1385,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
@@ -1481,13 +1400,13 @@
         <v>7</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F59" s="4"/>
     </row>
@@ -1496,13 +1415,13 @@
         <v>7</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F60" s="4"/>
     </row>
@@ -1511,13 +1430,13 @@
         <v>7</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F61" s="4"/>
     </row>
@@ -1526,7 +1445,7 @@
         <v>7</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>9</v>
@@ -1541,13 +1460,13 @@
         <v>7</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F63" s="4"/>
     </row>
@@ -1556,7 +1475,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
@@ -1571,7 +1490,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>9</v>
@@ -1586,7 +1505,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>9</v>
@@ -1601,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F67" s="4"/>
     </row>
@@ -1616,13 +1535,13 @@
         <v>7</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F68" s="4"/>
     </row>
@@ -1631,13 +1550,13 @@
         <v>7</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F69" s="4"/>
     </row>
@@ -1646,7 +1565,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>9</v>
@@ -1661,13 +1580,13 @@
         <v>7</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F71" s="4"/>
     </row>
@@ -1676,7 +1595,7 @@
         <v>7</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>9</v>
@@ -1691,7 +1610,7 @@
         <v>7</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>9</v>
@@ -1706,7 +1625,7 @@
         <v>7</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>9</v>
@@ -1721,13 +1640,13 @@
         <v>7</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F75" s="4"/>
     </row>
@@ -1736,13 +1655,13 @@
         <v>7</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F76" s="4"/>
     </row>
@@ -1751,13 +1670,13 @@
         <v>7</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F77" s="4"/>
     </row>
@@ -1766,13 +1685,13 @@
         <v>7</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F78" s="4"/>
     </row>
@@ -1781,7 +1700,7 @@
         <v>7</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>9</v>
@@ -1796,13 +1715,13 @@
         <v>7</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F80" s="4"/>
     </row>
@@ -1811,7 +1730,7 @@
         <v>7</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>9</v>
@@ -1826,7 +1745,7 @@
         <v>7</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>9</v>
@@ -1841,7 +1760,7 @@
         <v>7</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>9</v>
@@ -1856,13 +1775,13 @@
         <v>7</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F84" s="4"/>
     </row>
@@ -1871,13 +1790,13 @@
         <v>7</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F85" s="4"/>
     </row>
@@ -1886,13 +1805,13 @@
         <v>7</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F86" s="4"/>
     </row>
@@ -1901,7 +1820,7 @@
         <v>7</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>9</v>
@@ -1916,13 +1835,13 @@
         <v>7</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F88" s="4"/>
     </row>
@@ -1931,7 +1850,7 @@
         <v>7</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>9</v>
@@ -1946,7 +1865,7 @@
         <v>7</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>9</v>
@@ -1961,7 +1880,7 @@
         <v>7</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>9</v>
@@ -1976,13 +1895,13 @@
         <v>7</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F92" s="4"/>
     </row>
@@ -1991,13 +1910,13 @@
         <v>7</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F93" s="4"/>
     </row>
@@ -2006,13 +1925,13 @@
         <v>7</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F94" s="4"/>
     </row>
@@ -2021,7 +1940,7 @@
         <v>7</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>9</v>
@@ -2036,13 +1955,13 @@
         <v>7</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F96" s="4"/>
     </row>
@@ -2051,7 +1970,7 @@
         <v>7</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>9</v>
@@ -2066,7 +1985,7 @@
         <v>7</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>9</v>
@@ -2081,13 +2000,13 @@
         <v>7</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F99" s="4"/>
     </row>
@@ -2096,7 +2015,7 @@
         <v>7</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>9</v>
@@ -2111,13 +2030,13 @@
         <v>7</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F101" s="4"/>
     </row>
@@ -2126,13 +2045,13 @@
         <v>7</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F102" s="4"/>
     </row>
@@ -2141,13 +2060,13 @@
         <v>7</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F103" s="4"/>
     </row>
@@ -2156,7 +2075,7 @@
         <v>7</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>9</v>
@@ -2171,13 +2090,13 @@
         <v>7</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F105" s="4"/>
     </row>
@@ -2186,7 +2105,7 @@
         <v>7</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>9</v>
@@ -2201,7 +2120,7 @@
         <v>7</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>9</v>
@@ -2216,7 +2135,7 @@
         <v>7</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>9</v>
@@ -2231,13 +2150,13 @@
         <v>7</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F109" s="4"/>
     </row>
@@ -2246,13 +2165,13 @@
         <v>7</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F110" s="4"/>
     </row>
@@ -2261,13 +2180,13 @@
         <v>7</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F111" s="4"/>
     </row>
@@ -2276,7 +2195,7 @@
         <v>7</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>9</v>
@@ -2291,13 +2210,13 @@
         <v>7</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F113" s="4"/>
     </row>
@@ -2306,7 +2225,7 @@
         <v>7</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>9</v>
@@ -2322,7 +2241,7 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>9</v>
@@ -2338,7 +2257,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>9</v>
@@ -2354,13 +2273,13 @@
         <v>7</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F117" s="4"/>
       <c r="H117" s="4"/>
@@ -2370,13 +2289,13 @@
         <v>7</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F118" s="4"/>
     </row>
@@ -2385,13 +2304,13 @@
         <v>7</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F119" s="4"/>
     </row>
@@ -2400,13 +2319,13 @@
         <v>7</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F120" s="4"/>
     </row>
@@ -2415,7 +2334,7 @@
         <v>7</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>9</v>
@@ -2430,13 +2349,13 @@
         <v>7</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F122" s="4"/>
     </row>
@@ -2445,7 +2364,7 @@
         <v>7</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>9</v>
@@ -2460,7 +2379,7 @@
         <v>7</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>9</v>
@@ -2475,7 +2394,7 @@
         <v>7</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>9</v>
@@ -2490,13 +2409,13 @@
         <v>7</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F126" s="4"/>
     </row>
@@ -2505,13 +2424,13 @@
         <v>7</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F127" s="4"/>
     </row>
@@ -2520,13 +2439,13 @@
         <v>7</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F128" s="4"/>
     </row>
@@ -2535,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>9</v>
@@ -2550,13 +2469,13 @@
         <v>7</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F130" s="4"/>
     </row>
@@ -2565,7 +2484,7 @@
         <v>7</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>9</v>
@@ -2580,7 +2499,7 @@
         <v>7</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>9</v>
@@ -2595,7 +2514,7 @@
         <v>7</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>9</v>
@@ -2610,13 +2529,13 @@
         <v>7</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F134" s="4"/>
     </row>
@@ -2625,13 +2544,13 @@
         <v>7</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F135" s="4"/>
     </row>
@@ -2640,13 +2559,13 @@
         <v>7</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F136" s="4"/>
     </row>
@@ -2655,7 +2574,7 @@
         <v>7</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>9</v>
@@ -2670,13 +2589,13 @@
         <v>7</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F138" s="4"/>
     </row>
@@ -2685,7 +2604,7 @@
         <v>7</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>9</v>
@@ -2700,7 +2619,7 @@
         <v>7</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>9</v>
@@ -2715,13 +2634,13 @@
         <v>7</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F141" s="4"/>
     </row>
@@ -2730,7 +2649,7 @@
         <v>7</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D142" s="4" t="s">
         <v>9</v>
@@ -2745,13 +2664,13 @@
         <v>7</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D143" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F143" s="4"/>
     </row>
@@ -2760,13 +2679,13 @@
         <v>7</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F144" s="4"/>
     </row>
@@ -2775,13 +2694,13 @@
         <v>7</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F145" s="4"/>
     </row>
@@ -2790,7 +2709,7 @@
         <v>7</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>9</v>
@@ -2805,13 +2724,13 @@
         <v>7</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D147" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F147" s="4"/>
     </row>
@@ -2820,7 +2739,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D148" s="4" t="s">
         <v>9</v>
@@ -2835,7 +2754,7 @@
         <v>7</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D149" s="4" t="s">
         <v>9</v>
@@ -2850,7 +2769,7 @@
         <v>7</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D150" s="4" t="s">
         <v>9</v>
@@ -2865,13 +2784,13 @@
         <v>7</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D151" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F151" s="4"/>
     </row>
@@ -2880,13 +2799,13 @@
         <v>7</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D152" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F152" s="4"/>
     </row>
@@ -2895,13 +2814,13 @@
         <v>7</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D153" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F153" s="4"/>
     </row>
@@ -2910,7 +2829,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>9</v>
@@ -2925,13 +2844,13 @@
         <v>7</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F155" s="4"/>
     </row>
@@ -2940,7 +2859,7 @@
         <v>7</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D156" s="4" t="s">
         <v>9</v>
@@ -2955,7 +2874,7 @@
         <v>7</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D157" s="4" t="s">
         <v>9</v>
@@ -2970,7 +2889,7 @@
         <v>7</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="D158" s="4" t="s">
         <v>9</v>
@@ -2985,13 +2904,13 @@
         <v>7</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="D159" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F159" s="4"/>
     </row>
@@ -3000,13 +2919,13 @@
         <v>7</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F160" s="4"/>
     </row>
@@ -3015,13 +2934,13 @@
         <v>7</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D161" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F161" s="4"/>
     </row>
@@ -3030,13 +2949,13 @@
         <v>7</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D162" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F162" s="4"/>
     </row>
@@ -3045,7 +2964,7 @@
         <v>7</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>9</v>
@@ -3060,13 +2979,13 @@
         <v>7</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D164" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F164" s="4"/>
     </row>
@@ -3075,7 +2994,7 @@
         <v>7</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>9</v>
@@ -3090,7 +3009,7 @@
         <v>7</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D166" s="4" t="s">
         <v>9</v>
@@ -3105,7 +3024,7 @@
         <v>7</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D167" s="4" t="s">
         <v>9</v>
@@ -3120,13 +3039,13 @@
         <v>7</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D168" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F168" s="4"/>
     </row>
@@ -3135,13 +3054,13 @@
         <v>7</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D169" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F169" s="4"/>
     </row>
@@ -3150,13 +3069,13 @@
         <v>7</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D170" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F170" s="4"/>
     </row>
@@ -3165,7 +3084,7 @@
         <v>7</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>9</v>
@@ -3180,13 +3099,13 @@
         <v>7</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F172" s="4"/>
     </row>
@@ -3195,7 +3114,7 @@
         <v>7</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="D173" s="4" t="s">
         <v>9</v>
@@ -3210,7 +3129,7 @@
         <v>7</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="D174" s="4" t="s">
         <v>9</v>
@@ -3225,7 +3144,7 @@
         <v>7</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>9</v>
@@ -3240,13 +3159,13 @@
         <v>7</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D176" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E176" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F176" s="4"/>
     </row>
@@ -3255,13 +3174,13 @@
         <v>7</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D177" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F177" s="4"/>
     </row>
@@ -3270,13 +3189,13 @@
         <v>7</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F178" s="4"/>
     </row>
@@ -3285,7 +3204,7 @@
         <v>7</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D179" s="4" t="s">
         <v>9</v>
@@ -3300,13 +3219,13 @@
         <v>7</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F180" s="4"/>
     </row>
@@ -3315,7 +3234,7 @@
         <v>7</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>9</v>
@@ -3330,7 +3249,7 @@
         <v>7</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D182" s="4" t="s">
         <v>9</v>
@@ -3345,13 +3264,13 @@
         <v>7</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D183" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F183" s="4"/>
     </row>
@@ -3360,7 +3279,7 @@
         <v>7</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D184" s="4" t="s">
         <v>9</v>
@@ -3375,13 +3294,13 @@
         <v>7</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D185" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F185" s="4"/>
     </row>
@@ -3390,13 +3309,13 @@
         <v>7</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D186" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F186" s="4"/>
     </row>
@@ -3405,13 +3324,13 @@
         <v>7</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D187" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F187" s="4"/>
     </row>
@@ -3420,7 +3339,7 @@
         <v>7</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="D188" s="4" t="s">
         <v>9</v>
@@ -3435,13 +3354,13 @@
         <v>7</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D189" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F189" s="4"/>
     </row>
@@ -3450,7 +3369,7 @@
         <v>7</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D190" s="4" t="s">
         <v>9</v>
@@ -3465,7 +3384,7 @@
         <v>7</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D191" s="4" t="s">
         <v>9</v>
@@ -3480,7 +3399,7 @@
         <v>7</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D192" s="4" t="s">
         <v>9</v>
@@ -3495,13 +3414,13 @@
         <v>7</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D193" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F193" s="4"/>
     </row>
@@ -3510,13 +3429,13 @@
         <v>7</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="D194" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F194" s="4"/>
     </row>
@@ -3525,13 +3444,13 @@
         <v>7</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D195" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F195" s="4"/>
     </row>
@@ -3540,7 +3459,7 @@
         <v>7</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="D196" s="4" t="s">
         <v>9</v>
@@ -3555,13 +3474,13 @@
         <v>7</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="D197" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F197" s="4"/>
     </row>
@@ -3570,7 +3489,7 @@
         <v>7</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="D198" s="4" t="s">
         <v>9</v>
@@ -3585,7 +3504,7 @@
         <v>7</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="D199" s="4" t="s">
         <v>9</v>
@@ -3600,7 +3519,7 @@
         <v>7</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D200" s="4" t="s">
         <v>9</v>
@@ -3615,13 +3534,13 @@
         <v>7</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D201" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F201" s="4"/>
     </row>
@@ -3630,13 +3549,13 @@
         <v>7</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="D202" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F202" s="4"/>
     </row>
@@ -3645,13 +3564,13 @@
         <v>7</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="D203" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F203" s="4"/>
     </row>
@@ -3660,13 +3579,13 @@
         <v>7</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="D204" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F204" s="4"/>
     </row>
@@ -3675,7 +3594,7 @@
         <v>7</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="D205" s="4" t="s">
         <v>9</v>
@@ -3690,13 +3609,13 @@
         <v>7</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="D206" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F206" s="4"/>
     </row>
@@ -3705,7 +3624,7 @@
         <v>7</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D207" s="4" t="s">
         <v>9</v>
@@ -3720,7 +3639,7 @@
         <v>7</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="D208" s="4" t="s">
         <v>9</v>
@@ -3735,7 +3654,7 @@
         <v>7</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="D209" s="4" t="s">
         <v>9</v>
@@ -3750,13 +3669,13 @@
         <v>7</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="D210" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E210" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F210" s="4"/>
     </row>
@@ -3765,13 +3684,13 @@
         <v>7</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="D211" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E211" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F211" s="4"/>
     </row>
@@ -3780,13 +3699,13 @@
         <v>7</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D212" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E212" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F212" s="4"/>
     </row>
@@ -3795,7 +3714,7 @@
         <v>7</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D213" s="4" t="s">
         <v>9</v>
@@ -3804,7 +3723,7 @@
         <v>10</v>
       </c>
       <c r="F213" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,7 +3731,7 @@
         <v>7</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D214" s="4" t="s">
         <v>9</v>
@@ -3821,7 +3740,7 @@
         <v>10</v>
       </c>
       <c r="F214" s="4" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3829,13 +3748,13 @@
         <v>7</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D215" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F215" s="4"/>
     </row>
@@ -3844,13 +3763,13 @@
         <v>7</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D216" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F216" s="4"/>
     </row>
@@ -3859,13 +3778,13 @@
         <v>7</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D217" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F217" s="4"/>
     </row>
@@ -3874,13 +3793,13 @@
         <v>7</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="D218" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F218" s="4"/>
     </row>
@@ -3889,13 +3808,13 @@
         <v>7</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="F219" s="4"/>
     </row>
@@ -3904,13 +3823,13 @@
         <v>7</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="E220" s="4" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="F220" s="4"/>
     </row>

</xml_diff>